<commit_message>
Testing zeros of xF and prediction outputs.
</commit_message>
<xml_diff>
--- a/database/AN_ep/expdata/2003.xlsx
+++ b/database/AN_ep/expdata/2003.xlsx
@@ -153,7 +153,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -163,6 +163,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -186,10 +190,10 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -480,8 +484,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
-        <v>0</v>
+      <c r="A10" s="3" t="n">
+        <v>0.001</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>3</v>

</xml_diff>